<commit_message>
5 person report added yasaman last person in turesday
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C823164A-38C1-459A-8F93-89D8EE558470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76333233-C9E5-40F4-B8C3-FBADCF17AC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -296,7 +296,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,6 +585,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,9 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -921,7 +921,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1259,27 +1259,39 @@
       <c r="U9"/>
     </row>
     <row r="10" spans="1:21" ht="26.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="33">
+      <c r="B10" s="34">
         <v>8</v>
       </c>
-      <c r="C10" s="33">
+      <c r="C10" s="34">
         <v>98522175</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
+      <c r="F10" s="36">
+        <v>100</v>
+      </c>
+      <c r="G10" s="37">
+        <v>100</v>
+      </c>
+      <c r="H10" s="37">
+        <v>100</v>
+      </c>
+      <c r="I10" s="37">
+        <v>88</v>
+      </c>
+      <c r="J10" s="37">
+        <v>70</v>
+      </c>
+      <c r="K10" s="38">
+        <v>100</v>
+      </c>
       <c r="L10" s="13"/>
       <c r="M10" s="7"/>
       <c r="N10"/>

</xml_diff>

<commit_message>
Hossein Bahrami Degree Added
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76333233-C9E5-40F4-B8C3-FBADCF17AC73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBF2E5D-043A-4C96-B9AD-368C4C908B14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59220017-CF7D-445A-B888-10DB4F1AF4F8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1455,12 +1455,24 @@
       <c r="E15" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F15" s="23"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="3"/>
+      <c r="F15" s="23">
+        <v>100</v>
+      </c>
+      <c r="G15" s="2">
+        <v>100</v>
+      </c>
+      <c r="H15" s="2">
+        <v>100</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0</v>
+      </c>
+      <c r="J15" s="2">
+        <v>90</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
       <c r="L15" s="13"/>
       <c r="M15" s="7"/>
       <c r="N15"/>

</xml_diff>

<commit_message>
Hedieh Eshaghi Degree Added
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBF2E5D-043A-4C96-B9AD-368C4C908B14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B41957-CE18-429C-913C-71F25439A93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59220017-CF7D-445A-B888-10DB4F1AF4F8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1093,12 +1093,24 @@
       <c r="E5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="3"/>
+      <c r="F5" s="23">
+        <v>100</v>
+      </c>
+      <c r="G5" s="2">
+        <v>100</v>
+      </c>
+      <c r="H5" s="2">
+        <v>100</v>
+      </c>
+      <c r="I5" s="2">
+        <v>95</v>
+      </c>
+      <c r="J5" s="2">
+        <v>100</v>
+      </c>
+      <c r="K5" s="3">
+        <v>100</v>
+      </c>
       <c r="L5" s="13"/>
       <c r="M5" s="7"/>
       <c r="N5"/>

</xml_diff>

<commit_message>
Ali Akhbari Degree Added
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B41957-CE18-429C-913C-71F25439A93A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC79583-BC98-484E-A718-2C548608ECB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -920,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59220017-CF7D-445A-B888-10DB4F1AF4F8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1434,12 +1434,24 @@
       <c r="E14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="3"/>
+      <c r="F14" s="23">
+        <v>100</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0</v>
+      </c>
+      <c r="J14" s="2">
+        <v>60</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
       <c r="L14" s="13"/>
       <c r="M14" s="7"/>
       <c r="N14"/>

</xml_diff>

<commit_message>
Houreh and Arshia Dergrees added with failed
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC79583-BC98-484E-A718-2C548608ECB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD4793A-0307-45DD-B48D-EABD3AF1153F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -214,7 +214,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,8 +286,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,6 +304,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -602,6 +615,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -920,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59220017-CF7D-445A-B888-10DB4F1AF4F8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1123,27 +1157,39 @@
       <c r="U5"/>
     </row>
     <row r="6" spans="1:21" ht="26.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="40">
         <v>4</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="40">
         <v>99521208</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="3"/>
+      <c r="F6" s="42">
+        <v>100</v>
+      </c>
+      <c r="G6" s="43">
+        <v>100</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="43">
+        <v>80</v>
+      </c>
+      <c r="K6" s="44" t="s">
+        <v>23</v>
+      </c>
       <c r="L6" s="13"/>
       <c r="M6" s="7"/>
       <c r="N6"/>
@@ -1189,27 +1235,39 @@
       <c r="U7"/>
     </row>
     <row r="8" spans="1:21" ht="26.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="40">
         <v>6</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="40">
         <v>98412004</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="3"/>
+      <c r="F8" s="42">
+        <v>100</v>
+      </c>
+      <c r="G8" s="43">
+        <v>100</v>
+      </c>
+      <c r="H8" s="43">
+        <v>100</v>
+      </c>
+      <c r="I8" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="J8" s="43">
+        <v>100</v>
+      </c>
+      <c r="K8" s="44">
+        <v>98</v>
+      </c>
       <c r="L8" s="13" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Amir Azadi Dergree Added with falied
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD4793A-0307-45DD-B48D-EABD3AF1153F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6C3664-1732-448A-854B-E9C0FDD800C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -294,7 +294,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -313,6 +313,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -502,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -636,6 +642,24 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -955,7 +979,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1202,27 +1226,39 @@
       <c r="U6"/>
     </row>
     <row r="7" spans="1:21" ht="26.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="47">
         <v>5</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="47">
         <v>99521046</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
+      <c r="F7" s="49">
+        <v>100</v>
+      </c>
+      <c r="G7" s="50">
+        <v>100</v>
+      </c>
+      <c r="H7" s="50" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="50">
+        <v>100</v>
+      </c>
+      <c r="J7" s="50">
+        <v>100</v>
+      </c>
+      <c r="K7" s="51">
+        <v>100</v>
+      </c>
       <c r="L7" s="13"/>
       <c r="M7" s="7"/>
       <c r="N7"/>
@@ -1266,7 +1302,7 @@
         <v>100</v>
       </c>
       <c r="K8" s="44">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="L8" s="13" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
MR Hassani Degree Added with failed
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99AC911-663C-432E-B880-E2F3E867C19C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577BBD86-58A1-41E4-B703-647AC738E390}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -508,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -660,6 +660,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -978,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59220017-CF7D-445A-B888-10DB4F1AF4F8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1457,27 +1460,39 @@
       <c r="U11"/>
     </row>
     <row r="12" spans="1:21" ht="26.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="40">
         <v>10</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="40">
         <v>99522293</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="3"/>
+      <c r="F12" s="42">
+        <v>100</v>
+      </c>
+      <c r="G12" s="43">
+        <v>95</v>
+      </c>
+      <c r="H12" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="43">
+        <v>93</v>
+      </c>
+      <c r="J12" s="43">
+        <v>85</v>
+      </c>
+      <c r="K12" s="44">
+        <v>100</v>
+      </c>
       <c r="L12" s="13"/>
       <c r="M12" s="7"/>
       <c r="N12"/>

</xml_diff>

<commit_message>
Abolfazl Degree Added & End of the meeting
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577BBD86-58A1-41E4-B703-647AC738E390}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CAE2C7-4025-42E8-A798-25B85AEF6714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -982,7 +982,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1121,12 +1121,24 @@
       <c r="E4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="3"/>
+      <c r="F4" s="23">
+        <v>100</v>
+      </c>
+      <c r="G4" s="2">
+        <v>100</v>
+      </c>
+      <c r="H4" s="2">
+        <v>100</v>
+      </c>
+      <c r="I4" s="2">
+        <v>100</v>
+      </c>
+      <c r="J4" s="2">
+        <v>100</v>
+      </c>
+      <c r="K4" s="3">
+        <v>100</v>
+      </c>
       <c r="L4" s="13"/>
       <c r="M4" s="7"/>
       <c r="N4"/>

</xml_diff>

<commit_message>
All fail is fixed
</commit_message>
<xml_diff>
--- a/ارایه تمرین 1 و 2.xlsx
+++ b/ارایه تمرین 1 و 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hessam-PC\Desktop\tamrin_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249960F9-3AD8-406E-9869-E8B1D7284F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FF6636-41EA-43C1-8AE5-ED465FAFAD34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3B93B080-0797-444D-B041-832826163AE2}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>#</t>
   </si>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59220017-CF7D-445A-B888-10DB4F1AF4F8}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.2" x14ac:dyDescent="0.3"/>
@@ -1220,17 +1220,17 @@
       <c r="G6" s="43">
         <v>100</v>
       </c>
-      <c r="H6" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="I6" s="43" t="s">
-        <v>23</v>
+      <c r="H6" s="43">
+        <v>78</v>
+      </c>
+      <c r="I6" s="43">
+        <v>3</v>
       </c>
       <c r="J6" s="43">
         <v>80</v>
       </c>
-      <c r="K6" s="44" t="s">
-        <v>23</v>
+      <c r="K6" s="44">
+        <v>3</v>
       </c>
       <c r="L6" s="13"/>
       <c r="M6" s="7"/>

</xml_diff>